<commit_message>
add Elliot's notes for GNG contrasts
</commit_message>
<xml_diff>
--- a/fMRI/fx/gng/prepost_analysis/gng-contrast-weights.xlsx
+++ b/fMRI/fx/gng/prepost_analysis/gng-contrast-weights.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadestasio/Desktop/REV_scripts/fMRI/fx/gng/prepost_analysis/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="440" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>'correct_risk_go'</t>
   </si>
@@ -81,6 +76,27 @@
   </si>
   <si>
     <t>instructions</t>
+  </si>
+  <si>
+    <t>*DON'T NEED TO WORRY ABOUT INCORRECT VS CORRECT</t>
+  </si>
+  <si>
+    <t>2_Risk&gt;Neutral</t>
+  </si>
+  <si>
+    <t>4_NoGoRisk&gt;GoRisk</t>
+  </si>
+  <si>
+    <t>3_RiskNoGo.v.Go&gt;NeutralNoGo.v.Go</t>
+  </si>
+  <si>
+    <t>5_NoGoNeutral&gt;GoNeutral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average pre, average post, average across, pre-post change, </t>
+  </si>
+  <si>
+    <t>*At group level, you can flip contrasts (e.g. look at Go&gt;NoGo as sanity check for motor activity)</t>
   </si>
 </sst>
 </file>
@@ -129,8 +145,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -162,7 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -176,6 +200,10 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -189,6 +217,10 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -244,7 +276,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -279,7 +311,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -456,7 +488,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -464,15 +496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:S8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -492,7 +524,7 @@
     <col min="18" max="18" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -551,7 +583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -611,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -671,7 +703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -730,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -789,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -848,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -907,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -966,8 +998,63 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:19">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>